<commit_message>
[UPDATE][model] Add simulation index to the data modle and calculation
</commit_message>
<xml_diff>
--- a/outputs/pool_data.xlsx
+++ b/outputs/pool_data.xlsx
@@ -34,7 +34,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="7">
+  <si>
+    <t>id_sim</t>
+  </si>
+  <si>
+    <t>id_pool</t>
+  </si>
   <si>
     <t>math_res_opening</t>
   </si>
@@ -46,9 +52,6 @@
   </si>
   <si>
     <t>spread</t>
-  </si>
-  <si>
-    <t>id_pool</t>
   </si>
   <si>
     <t>ps_rate</t>
@@ -409,16 +412,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,16 +431,22 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -448,21 +454,125 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -473,16 +583,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,46 +603,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>260072499</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>259965626</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -546,16 +775,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,47 +795,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>260072499</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>259965626</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -619,16 +967,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,47 +987,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>260072499</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>259965626</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -692,16 +1159,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,47 +1179,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
+        <v>260072499</v>
+      </c>
+      <c r="E2">
+        <v>260072499</v>
+      </c>
+      <c r="F2">
         <v>192453649.26</v>
       </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
+        <v>259965626</v>
+      </c>
+      <c r="E3">
+        <v>259965626</v>
+      </c>
+      <c r="F3">
         <v>191074735.11</v>
       </c>
-      <c r="E3">
-        <v>0.005</v>
-      </c>
-      <c r="F3">
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -765,16 +1351,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,47 +1371,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>192453649.26</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>192453649.26</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
+        <v>192453649.26</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>191074735.11</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>191074735.11</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>191074735.11</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -838,16 +1543,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,47 +1563,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>192453649.26</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>192453649.26</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
+        <v>192453649.26</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>191074735.11</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>191074735.11</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>191074735.11</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -911,16 +1735,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,47 +1755,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>192453649.26</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>192453649.26</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
+        <v>192453649.26</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>191074735.11</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>191074735.11</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>191074735.11</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -984,16 +1927,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,47 +1947,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>192453649.26</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>192453649.26</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>192453649.26</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>192453649.26</v>
       </c>
       <c r="F2">
+        <v>192453649.26</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>191074735.11</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>191074735.11</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>191074735.11</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>195054374.25</v>
       </c>
       <c r="F3">
+        <v>191074735.11</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>-0.265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>234065249.1</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>191074735.11</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>193674391.37</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>-0.09999999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>232669235.27</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>-0.105</v>
       </c>
     </row>
   </sheetData>
@@ -1057,16 +2119,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,47 +2139,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>192453649.26</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>192453649.26</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>192453649.26</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>192453649.26</v>
       </c>
       <c r="F2">
+        <v>192453649.26</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>0.08000000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>191074735.11</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>191074735.11</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>191074735.11</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>195054374.25</v>
       </c>
       <c r="F3">
+        <v>191074735.11</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>0.07500000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>234065249.1</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>191074735.11</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>193674391.37</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>232669235.27</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>0.195</v>
       </c>
     </row>
   </sheetData>
@@ -1130,16 +2311,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1153,47 +2331,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>192453649.26</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>192453649.26</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>192453649.26</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>192453649.26</v>
       </c>
       <c r="F2">
+        <v>192453649.26</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>0.08000000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>191074735.11</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>191074735.11</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>191074735.11</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>195054374.25</v>
       </c>
       <c r="F3">
+        <v>191074735.11</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>0.07500000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>234065249.1</v>
+      </c>
+      <c r="F4">
+        <v>195054374.25</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>191074735.11</v>
+      </c>
+      <c r="F5">
+        <v>193674391.37</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>193674391.37</v>
+      </c>
+      <c r="F6">
+        <v>234065249.1</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>232669235.27</v>
+      </c>
+      <c r="F7">
+        <v>232669235.27</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>0.195</v>
       </c>
     </row>
   </sheetData>
@@ -1203,16 +2503,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1225,16 +2522,22 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1242,21 +2545,125 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -1267,16 +2674,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,47 +2694,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>192453649.26</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>192453649.26</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>207849941.2008</v>
       </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>0.08000000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>191074735.11</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>191074735.11</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>205405340.24325</v>
       </c>
-      <c r="E3">
-        <v>0.005</v>
-      </c>
-      <c r="F3">
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>0.07500000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>195054374.25</v>
+      </c>
+      <c r="E4">
+        <v>195054374.25</v>
+      </c>
+      <c r="F4">
+        <v>128735887.005</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>193674391.37</v>
+      </c>
+      <c r="E5">
+        <v>193674391.37</v>
+      </c>
+      <c r="F5">
+        <v>126856726.34735</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>234065249.1</v>
+      </c>
+      <c r="E6">
+        <v>234065249.1</v>
+      </c>
+      <c r="F6">
+        <v>280878298.92</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>232669235.27</v>
+      </c>
+      <c r="E7">
+        <v>232669235.27</v>
+      </c>
+      <c r="F7">
+        <v>278039736.1476499</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>0.195</v>
       </c>
     </row>
   </sheetData>
@@ -1340,16 +2866,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1363,47 +2886,169 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>207849941.2008</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>192453649.26</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>207849941.2008</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>192453649.26</v>
       </c>
       <c r="F2">
+        <v>207849941.2008</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
         <v>0.08000000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>205405340.24325</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>191074735.11</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>205405340.24325</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>191074735.11</v>
       </c>
       <c r="F3">
+        <v>205405340.24325</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
         <v>0.07500000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>128735887.005</v>
+      </c>
+      <c r="E4">
+        <v>195054374.25</v>
+      </c>
+      <c r="F4">
+        <v>128735887.005</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>-0.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>126856726.34735</v>
+      </c>
+      <c r="E5">
+        <v>193674391.37</v>
+      </c>
+      <c r="F5">
+        <v>126856726.34735</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>-0.345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>280878298.92</v>
+      </c>
+      <c r="E6">
+        <v>234065249.1</v>
+      </c>
+      <c r="F6">
+        <v>280878298.92</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>278039736.1476499</v>
+      </c>
+      <c r="E7">
+        <v>232669235.27</v>
+      </c>
+      <c r="F7">
+        <v>278039736.1476499</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
+        <v>0.195</v>
       </c>
     </row>
   </sheetData>
@@ -1413,16 +3058,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1435,38 +3077,148 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>260072499</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
+        <v>260072499</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>259965626</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -1477,16 +3229,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1500,46 +3249,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>260072499</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>259965626</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -1550,16 +3421,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1573,46 +3441,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>260072499</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>259965626</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -1623,16 +3613,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1646,46 +3633,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -1696,16 +3805,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1719,46 +3825,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -1769,16 +3997,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1792,46 +4017,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -1842,16 +4189,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1865,46 +4209,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>260072499</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>260072499</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>260072499</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>260072499</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>260072499</v>
+      </c>
+      <c r="G2">
+        <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>259965626</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>259965626</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>259965626</v>
       </c>
       <c r="E3">
-        <v>0.005</v>
+        <v>259965626</v>
       </c>
       <c r="F3">
+        <v>259965626</v>
+      </c>
+      <c r="G3">
+        <v>0.005</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>260072499</v>
+      </c>
+      <c r="E4">
+        <v>260072499</v>
+      </c>
+      <c r="F4">
+        <v>260072499</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>259965626</v>
+      </c>
+      <c r="E5">
+        <v>259965626</v>
+      </c>
+      <c r="F5">
+        <v>259965626</v>
+      </c>
+      <c r="G5">
+        <v>0.005</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>260072499</v>
+      </c>
+      <c r="E6">
+        <v>260072499</v>
+      </c>
+      <c r="F6">
+        <v>260072499</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>259965626</v>
+      </c>
+      <c r="E7">
+        <v>259965626</v>
+      </c>
+      <c r="F7">
+        <v>259965626</v>
+      </c>
+      <c r="G7">
+        <v>0.005</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>

</xml_diff>